<commit_message>
SS : Add security fund in Associate SS : Add crypto address in ID MISC : Remove linebreak check in Linter
</commit_message>
<xml_diff>
--- a/Data/FiMs ID.xlsx
+++ b/Data/FiMs ID.xlsx
@@ -1,7 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
+  <bookViews>
+    <workbookView activeTab="0"/>
+  </bookViews>
   <sheets>
     <sheet state="visible" name="ID" sheetId="1" r:id="rId4"/>
   </sheets>
@@ -116,37 +119,61 @@
   <si>
     <t>Yes</t>
   </si>
+  <si>
+    <t>Crypto Address
+CCLcWAJX6fubUqGyZWz8dyUGEddRj8h4XZZCNSDzMVx4</t>
+  </si>
+  <si>
+    <t>Crypto Address</t>
+  </si>
+  <si>
+    <t>CCLcWAJX6fubUqGyZWz8dyUGEddRj8h4XZZCNSDzMVx4</t>
+  </si>
+  <si>
+    <t>CCLcWAJX6fubUqGyZWz8dyUGEddRj8h4XZZCNSD</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="2" mc:Ignorable="x14ac">
+  <numFmts count="10">
+    <numFmt numFmtId="5" formatCode="&quot;$&quot;#,##0_);(&quot;$&quot;#,##0)"/>
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red](&quot;$&quot;#,##0)"/>
+    <numFmt numFmtId="7" formatCode="&quot;$&quot;#,##0.00_);(&quot;$&quot;#,##0.00)"/>
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red](&quot;$&quot;#,##0.00)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* (#,##0);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* (#,##0);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* (#,##0.00);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* (#,##0.00);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="#,##0.00\ [$€-1]"/>
     <numFmt numFmtId="165" formatCode="dd/MM/yyyy"/>
   </numFmts>
   <fonts count="4">
     <font>
-      <sz val="10.0"/>
+      <name val="Arial"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
+      <sz val="10"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="Arial"/>
       <b/>
       <i/>
-      <color theme="1"/>
-      <name val="Arial"/>
+      <color rgb="FF000000"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <color theme="1"/>
       <name val="Arial"/>
+      <color rgb="FF000000"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <color theme="1"/>
       <name val="Arial"/>
+      <color rgb="FF000000"/>
+      <sz val="12"/>
     </font>
   </fonts>
   <fills count="5">
@@ -184,42 +211,40 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="3" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="3" numFmtId="165" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
 </styleSheet>
@@ -424,34 +449,34 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FF00FF00"/>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2.0" ySplit="1.0" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="C1" sqref="C1" pane="topRight"/>
-      <selection activeCell="A2" sqref="A2" pane="bottomLeft"/>
-      <selection activeCell="C2" sqref="C2" pane="bottomRight"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="12.63" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="5.38"/>
-    <col customWidth="1" min="3" max="3" width="21.38"/>
-    <col customWidth="1" min="7" max="7" width="9.38"/>
-    <col customWidth="1" min="8" max="8" width="20.88"/>
-    <col customWidth="1" min="9" max="9" width="19.38"/>
-    <col customWidth="1" min="10" max="10" width="10.63"/>
-    <col customWidth="1" min="11" max="11" width="21.13"/>
-    <col customWidth="1" min="12" max="12" width="27.25"/>
-    <col customWidth="1" min="13" max="13" width="24.13"/>
-    <col customWidth="1" min="14" max="14" width="21.75"/>
-    <col customWidth="1" min="15" max="15" width="9.38"/>
-    <col customWidth="1" hidden="1" min="16" max="16" width="8.88"/>
-    <col customWidth="1" hidden="1" min="17" max="17" width="7.5"/>
+    <col min="1" max="1" width="5.38" customWidth="1"/>
+    <col min="3" max="3" width="21.38" customWidth="1"/>
+    <col min="7" max="7" width="9.38" customWidth="1"/>
+    <col min="8" max="8" width="20.88" customWidth="1"/>
+    <col min="9" max="9" width="19.38" customWidth="1"/>
+    <col min="10" max="10" width="10.63" customWidth="1"/>
+    <col min="11" max="11" width="21.13" customWidth="1"/>
+    <col min="12" max="12" width="27.25" customWidth="1"/>
+    <col min="13" max="13" width="24.13" customWidth="1"/>
+    <col min="15" max="15" width="21.75" customWidth="1"/>
+    <col min="16" max="16" width="9.38" customWidth="1"/>
+    <col min="17" max="17" width="8.88" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="7.5" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -494,16 +519,19 @@
       <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="O1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>16</v>
       </c>
     </row>
@@ -528,7 +556,7 @@
         <v>21</v>
       </c>
       <c r="G2" s="8">
-        <v>36892.0</v>
+        <v>36892</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>22</v>
@@ -537,7 +565,7 @@
         <v>23</v>
       </c>
       <c r="J2" s="6">
-        <v>12345.0</v>
+        <v>12345</v>
       </c>
       <c r="K2" s="6" t="s">
         <v>22</v>
@@ -548,14 +576,17 @@
       <c r="M2" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="N2" s="9" t="s">
+      <c r="N2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="O2" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="P2" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="P2" s="6"/>
       <c r="Q2" s="6"/>
+      <c r="R2" s="6"/>
     </row>
   </sheetData>
   <drawing r:id="rId2"/>

</xml_diff>